<commit_message>
Milestone: fix investment inputs?
Investment runs finally seem to work without infeasibilities. Still need to decide and configure actual runs, but this should work as a start?
</commit_message>
<xml_diff>
--- a/src_files/data_files/gg-smr-scenario-changes.xlsx
+++ b/src_files/data_files/gg-smr-scenario-changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6426D96C-7E84-4F58-BDA6-B5B2FD23172F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F3E432-4FB8-4F37-917E-DC0DC8FB16E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="17880" windowWidth="29040" windowHeight="15720" tabRatio="862" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="17880" windowWidth="29040" windowHeight="15720" tabRatio="862" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="20" r:id="rId1"/>
@@ -1284,9 +1284,6 @@
     <t>rampUpCost</t>
   </si>
   <si>
-    <t>upperLimitCapacityRatio_input1</t>
-  </si>
-  <si>
     <t>useTimeseriesAvailability</t>
   </si>
   <si>
@@ -1384,6 +1381,9 @@
   </si>
   <si>
     <t>capacity_output1_raw</t>
+  </si>
+  <si>
+    <t>upperLimitCapacityRatio</t>
   </si>
 </sst>
 </file>
@@ -4354,18 +4354,18 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>340</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4391,18 +4391,18 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>343</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>345</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -14725,8 +14725,8 @@
   </sheetPr>
   <dimension ref="A1:O226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="F130" sqref="F130"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14766,7 +14766,7 @@
         <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>252</v>
@@ -27970,10 +27970,10 @@
         <v>196</v>
       </c>
       <c r="AH1" s="101" t="s">
+        <v>321</v>
+      </c>
+      <c r="AI1" s="101" t="s">
         <v>322</v>
-      </c>
-      <c r="AI1" s="101" t="s">
-        <v>323</v>
       </c>
       <c r="AJ1" s="101" t="s">
         <v>27</v>
@@ -27981,7 +27981,7 @@
     </row>
     <row r="2" spans="1:36" s="105" customFormat="1">
       <c r="A2" s="101" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B2" s="101">
         <v>1</v>
@@ -27990,13 +27990,13 @@
         <v>260</v>
       </c>
       <c r="D2" s="101" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E2" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G2" s="104"/>
       <c r="H2" s="102">
@@ -28078,7 +28078,7 @@
     </row>
     <row r="3" spans="1:36" s="107" customFormat="1">
       <c r="A3" s="101" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B3" s="101">
         <v>1</v>
@@ -28087,13 +28087,13 @@
         <v>260</v>
       </c>
       <c r="D3" s="101" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E3" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F3" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G3" s="106"/>
       <c r="H3" s="102">
@@ -28175,7 +28175,7 @@
     </row>
     <row r="4" spans="1:36" s="106" customFormat="1">
       <c r="A4" s="101" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B4" s="101">
         <v>1</v>
@@ -28184,13 +28184,13 @@
         <v>260</v>
       </c>
       <c r="D4" s="101" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E4" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F4" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H4" s="102">
         <v>0.33</v>
@@ -28269,12 +28269,12 @@
       <c r="AH4" s="101"/>
       <c r="AI4" s="101"/>
       <c r="AJ4" s="106" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:36" s="107" customFormat="1">
       <c r="A5" s="101" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5" s="101">
         <v>1</v>
@@ -28283,13 +28283,13 @@
         <v>260</v>
       </c>
       <c r="D5" s="101" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E5" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F5" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G5" s="101"/>
       <c r="H5" s="102">
@@ -28371,7 +28371,7 @@
     </row>
     <row r="6" spans="1:36" s="107" customFormat="1">
       <c r="A6" s="101" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6" s="101">
         <v>1</v>
@@ -28380,13 +28380,13 @@
         <v>260</v>
       </c>
       <c r="D6" s="101" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E6" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F6" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G6" s="104"/>
       <c r="H6" s="102">
@@ -28468,7 +28468,7 @@
     </row>
     <row r="7" spans="1:36">
       <c r="A7" s="101" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B7" s="101">
         <v>1</v>
@@ -28477,13 +28477,13 @@
         <v>260</v>
       </c>
       <c r="D7" s="101" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E7" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F7" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H7" s="102">
         <v>0.38</v>
@@ -28558,12 +28558,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ7" s="101" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:36">
       <c r="A8" s="101" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B8" s="101">
         <v>1</v>
@@ -28572,13 +28572,13 @@
         <v>260</v>
       </c>
       <c r="D8" s="101" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E8" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F8" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G8" s="104"/>
       <c r="H8" s="102">
@@ -28654,12 +28654,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ8" s="101" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:36">
       <c r="A9" s="101" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B9" s="101">
         <v>1</v>
@@ -28668,16 +28668,16 @@
         <v>261</v>
       </c>
       <c r="D9" s="101" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E9" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F9" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G9" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H9" s="102">
         <v>0.61</v>
@@ -28762,7 +28762,7 @@
     </row>
     <row r="10" spans="1:36">
       <c r="A10" s="101" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B10" s="101">
         <v>1</v>
@@ -28771,16 +28771,16 @@
         <v>261</v>
       </c>
       <c r="D10" s="101" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E10" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F10" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G10" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H10" s="102">
         <v>0.75</v>
@@ -28865,7 +28865,7 @@
     </row>
     <row r="11" spans="1:36">
       <c r="A11" s="101" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B11" s="101">
         <v>1</v>
@@ -28874,16 +28874,16 @@
         <v>261</v>
       </c>
       <c r="D11" s="101" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E11" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G11" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H11" s="102">
         <v>0.89</v>
@@ -28966,12 +28966,12 @@
       <c r="AH11" s="104"/>
       <c r="AI11" s="104"/>
       <c r="AJ11" s="106" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:36">
       <c r="A12" s="101" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B12" s="101">
         <v>1</v>
@@ -28980,16 +28980,16 @@
         <v>261</v>
       </c>
       <c r="D12" s="101" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E12" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F12" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G12" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H12" s="102">
         <v>0.92</v>
@@ -29074,7 +29074,7 @@
     </row>
     <row r="13" spans="1:36">
       <c r="A13" s="101" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B13" s="101">
         <v>1</v>
@@ -29083,16 +29083,16 @@
         <v>261</v>
       </c>
       <c r="D13" s="101" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E13" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G13" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H13" s="102">
         <v>0.94</v>
@@ -29177,7 +29177,7 @@
     </row>
     <row r="14" spans="1:36">
       <c r="A14" s="101" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B14" s="101">
         <v>1</v>
@@ -29186,16 +29186,16 @@
         <v>261</v>
       </c>
       <c r="D14" s="101" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E14" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G14" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H14" s="102">
         <v>0.92</v>
@@ -29276,12 +29276,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ14" s="101" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:36">
       <c r="A15" s="101" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B15" s="101">
         <v>1</v>
@@ -29290,16 +29290,16 @@
         <v>261</v>
       </c>
       <c r="D15" s="101" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E15" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G15" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H15" s="102">
         <v>0.94</v>
@@ -29380,12 +29380,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ15" s="101" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:36">
       <c r="A16" s="101" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B16" s="101">
         <v>1</v>
@@ -29394,13 +29394,13 @@
         <v>262</v>
       </c>
       <c r="D16" s="101" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E16" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G16" s="108"/>
       <c r="H16" s="102">
@@ -29478,7 +29478,7 @@
     </row>
     <row r="17" spans="1:36">
       <c r="A17" s="101" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B17" s="101">
         <v>1</v>
@@ -29487,13 +29487,13 @@
         <v>262</v>
       </c>
       <c r="D17" s="101" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E17" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G17" s="106"/>
       <c r="H17" s="102">
@@ -29573,7 +29573,7 @@
     </row>
     <row r="18" spans="1:36" s="104" customFormat="1">
       <c r="A18" s="101" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B18" s="101">
         <v>1</v>
@@ -29582,13 +29582,13 @@
         <v>262</v>
       </c>
       <c r="D18" s="101" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E18" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G18" s="106"/>
       <c r="H18" s="102">
@@ -29668,12 +29668,12 @@
       <c r="AH18" s="106"/>
       <c r="AI18" s="106"/>
       <c r="AJ18" s="106" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:36" s="109" customFormat="1">
       <c r="A19" s="101" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B19" s="101">
         <v>1</v>
@@ -29682,13 +29682,13 @@
         <v>262</v>
       </c>
       <c r="D19" s="101" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E19" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F19" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G19" s="101"/>
       <c r="H19" s="102">
@@ -29770,7 +29770,7 @@
     </row>
     <row r="20" spans="1:36" s="104" customFormat="1">
       <c r="A20" s="101" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B20" s="101">
         <v>1</v>
@@ -29779,13 +29779,13 @@
         <v>262</v>
       </c>
       <c r="D20" s="101" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E20" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F20" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H20" s="102">
         <v>0.95</v>
@@ -29864,7 +29864,7 @@
     </row>
     <row r="21" spans="1:36">
       <c r="A21" s="101" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B21" s="101">
         <v>1</v>
@@ -29873,13 +29873,13 @@
         <v>262</v>
       </c>
       <c r="D21" s="101" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E21" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F21" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H21" s="102">
         <v>0.93</v>
@@ -29954,12 +29954,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ21" s="101" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22" spans="1:36">
       <c r="A22" s="101" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B22" s="101">
         <v>1</v>
@@ -29968,13 +29968,13 @@
         <v>262</v>
       </c>
       <c r="D22" s="101" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E22" s="101" t="s">
         <v>28</v>
       </c>
       <c r="F22" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G22" s="104"/>
       <c r="H22" s="102">
@@ -30050,7 +30050,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ22" s="101" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23" spans="1:36">
@@ -30990,8 +30990,11 @@
   </sheetPr>
   <dimension ref="A1:AT9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AT1" sqref="AT1:AT1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31000,7 +31003,7 @@
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="51.75">
+    <row r="1" spans="1:46" ht="39">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -31107,10 +31110,10 @@
         <v>313</v>
       </c>
       <c r="AJ1" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="AK1" s="4" t="s">
         <v>314</v>
-      </c>
-      <c r="AK1" s="4" t="s">
-        <v>315</v>
       </c>
       <c r="AL1" s="4" t="s">
         <v>27</v>
@@ -31157,10 +31160,10 @@
       <c r="H2" s="95"/>
       <c r="I2" s="95"/>
       <c r="J2" s="95" t="s">
+        <v>315</v>
+      </c>
+      <c r="K2" s="95" t="s">
         <v>316</v>
-      </c>
-      <c r="K2" s="95" t="s">
-        <v>317</v>
       </c>
       <c r="L2" s="95"/>
       <c r="M2" s="95"/>
@@ -31212,7 +31215,9 @@
       <c r="AI2" s="95">
         <v>0</v>
       </c>
-      <c r="AJ2" s="95"/>
+      <c r="AJ2" s="95">
+        <v>4</v>
+      </c>
       <c r="AK2" s="95"/>
       <c r="AM2" s="17">
         <v>1</v>
@@ -31259,10 +31264,10 @@
       <c r="H3" s="95"/>
       <c r="I3" s="95"/>
       <c r="J3" s="95" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L3" s="95"/>
       <c r="M3" s="95"/>
@@ -31314,9 +31319,6 @@
       <c r="AI3" s="95">
         <v>0</v>
       </c>
-      <c r="AJ3" s="95">
-        <v>4</v>
-      </c>
       <c r="AK3" s="95"/>
       <c r="AL3" s="96"/>
       <c r="AM3">
@@ -31358,10 +31360,10 @@
         <v>240</v>
       </c>
       <c r="J4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O4">
         <v>0.98</v>
@@ -31446,10 +31448,10 @@
       <c r="H5" s="86"/>
       <c r="I5" s="86"/>
       <c r="J5" s="86" t="s">
+        <v>317</v>
+      </c>
+      <c r="K5" s="86" t="s">
         <v>318</v>
-      </c>
-      <c r="K5" s="86" t="s">
-        <v>319</v>
       </c>
       <c r="L5" s="86"/>
       <c r="M5" s="86"/>
@@ -31501,7 +31503,9 @@
       <c r="AI5" s="86">
         <v>0</v>
       </c>
-      <c r="AJ5" s="86"/>
+      <c r="AJ5" s="86">
+        <v>10</v>
+      </c>
       <c r="AK5" s="86"/>
       <c r="AL5" s="97"/>
       <c r="AM5">
@@ -31548,10 +31552,10 @@
       <c r="H6" s="86"/>
       <c r="I6" s="86"/>
       <c r="J6" s="86" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K6" s="86" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L6" s="86"/>
       <c r="M6" s="86"/>
@@ -31603,9 +31607,6 @@
       <c r="AI6" s="86">
         <v>0</v>
       </c>
-      <c r="AJ6" s="86">
-        <v>10</v>
-      </c>
       <c r="AK6" s="86"/>
       <c r="AL6" s="86"/>
       <c r="AM6" s="17">
@@ -31648,13 +31649,13 @@
         <v>189</v>
       </c>
       <c r="G7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J7" s="97" t="s">
         <v>157</v>
       </c>
       <c r="K7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -31733,13 +31734,13 @@
         <v>190</v>
       </c>
       <c r="G8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J8" s="97" t="s">
         <v>157</v>
       </c>
       <c r="K8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -31825,7 +31826,7 @@
         <v>157</v>
       </c>
       <c r="K9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O9">
         <v>1</v>

</xml_diff>

<commit_message>
Force warm starts to obey Backbone input data checks.
</commit_message>
<xml_diff>
--- a/src_files/data_files/gg-smr-scenario-changes.xlsx
+++ b/src_files/data_files/gg-smr-scenario-changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE66A49-BDFE-4635-934B-3688D2ECDF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533507E0-B0E9-4D0D-9F3C-22A166BFBF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="17880" windowWidth="29040" windowHeight="15720" tabRatio="862" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="862" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="20" r:id="rId1"/>
@@ -1401,7 +1401,7 @@
     <t>A mix of `nucLow` and `nucHigh` always sampling the disadvantageous parameter values.</t>
   </si>
   <si>
-    <t>Replicate data of interest from `unittypedata_nuclear-lwr-smr.xlsx` to manually override `unitSize`. (Needs to duplicate all parameters for now due to NE-model data processing oversights) (Also currently removes `cV` due to Backbone investment input data preprocessing limitations)</t>
+    <t>Replicate data of interest from `unittypedata_nuclear-lwr-smr.xlsx` to manually override `unitSize`. (Needs to duplicate all parameters for now due to NE-model data processing oversights) (Also currently removes `cV` due to Backbone investment input data preprocessing limitations, as well as forcing `minShutDownHours` &gt;= `startWarmAfterXHours`)</t>
   </si>
 </sst>
 </file>
@@ -4190,8 +4190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFA71A91-038D-4743-9A24-5EE3CD503F37}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14692,7 +14692,7 @@
   </sheetPr>
   <dimension ref="A1:O226"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -27802,10 +27802,10 @@
   <dimension ref="A1:AJ28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA3" sqref="AA3:AA28"/>
+      <selection pane="bottomRight" activeCell="W25" sqref="W25:W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -28467,8 +28467,8 @@
       <c r="V7">
         <v>50</v>
       </c>
-      <c r="W7">
-        <v>36</v>
+      <c r="W7" s="98">
+        <v>96</v>
       </c>
       <c r="X7">
         <v>144</v>
@@ -28562,8 +28562,8 @@
       <c r="V8">
         <v>30.25</v>
       </c>
-      <c r="W8">
-        <v>33</v>
+      <c r="W8" s="98">
+        <v>55</v>
       </c>
       <c r="X8">
         <v>132</v>
@@ -29364,8 +29364,8 @@
       <c r="V16">
         <v>61</v>
       </c>
-      <c r="W16">
-        <v>36</v>
+      <c r="W16" s="98">
+        <v>96</v>
       </c>
       <c r="X16">
         <v>144</v>
@@ -29468,8 +29468,8 @@
       <c r="V17">
         <v>36.33</v>
       </c>
-      <c r="W17">
-        <v>33</v>
+      <c r="W17" s="98">
+        <v>55</v>
       </c>
       <c r="X17">
         <v>132</v>
@@ -30234,8 +30234,8 @@
       <c r="V25">
         <v>25</v>
       </c>
-      <c r="W25">
-        <v>36</v>
+      <c r="W25" s="98">
+        <v>96</v>
       </c>
       <c r="X25">
         <v>144</v>
@@ -30329,8 +30329,8 @@
       <c r="V26">
         <v>15.25</v>
       </c>
-      <c r="W26">
-        <v>32</v>
+      <c r="W26" s="98">
+        <v>53</v>
       </c>
       <c r="X26">
         <v>126</v>

</xml_diff>

<commit_message>
Very minor data comments
</commit_message>
<xml_diff>
--- a/src_files/data_files/gg-smr-scenario-changes.xlsx
+++ b/src_files/data_files/gg-smr-scenario-changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533507E0-B0E9-4D0D-9F3C-22A166BFBF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC328F0-5165-4EF8-8CA6-02D9BFB1C28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="862" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="862" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="20" r:id="rId1"/>
@@ -315,7 +315,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3469" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3474" uniqueCount="355">
   <si>
     <t>Country</t>
   </si>
@@ -1167,9 +1167,6 @@
     <t>TEMPLATE</t>
   </si>
   <si>
-    <t>Check TYNDP2024 CAPEX and OPEX cost assumtpions, and use them for wind/solar investments.</t>
-  </si>
-  <si>
     <t>ETS-CO2</t>
   </si>
   <si>
@@ -1383,9 +1380,6 @@
     <t>Do I need to include pessimistic and worst-case scenarios for nuclear parameters to see if the investments vanish?</t>
   </si>
   <si>
-    <t>2025-09-18</t>
-  </si>
-  <si>
     <t>Reverts TYNDP2024 "National Trends" 2040 scenario unit capacities back to their 2030 counterparts and caps investments into the desired technologies. Needs to include rounding, as Backbone investment options need to be integer multiples of assumed unit size just to be safe.</t>
   </si>
   <si>
@@ -1402,6 +1396,15 @@
   </si>
   <si>
     <t>Replicate data of interest from `unittypedata_nuclear-lwr-smr.xlsx` to manually override `unitSize`. (Needs to duplicate all parameters for now due to NE-model data processing oversights) (Also currently removes `cV` due to Backbone investment input data preprocessing limitations, as well as forcing `minShutDownHours` &gt;= `startWarmAfterXHours`)</t>
+  </si>
+  <si>
+    <t>Check TYNDP2024 CAPEX and OPEX cost assumptions, and use them for wind/solar investments.</t>
+  </si>
+  <si>
+    <t>DEA data</t>
+  </si>
+  <si>
+    <t>2025-10-09</t>
   </si>
 </sst>
 </file>
@@ -4190,8 +4193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFA71A91-038D-4743-9A24-5EE3CD503F37}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4230,7 +4233,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4263,7 +4266,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="D11" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4298,12 +4301,12 @@
     </row>
     <row r="19" spans="1:3">
       <c r="C19" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="C20" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -4316,23 +4319,23 @@
         <v>65</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>336</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -4358,18 +4361,18 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>338</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>340</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -4401,7 +4404,7 @@
         <v>274</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>275</v>
+        <v>352</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -7402,8 +7405,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q354"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J358" sqref="J358"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K354" sqref="K354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
@@ -14692,7 +14695,7 @@
   </sheetPr>
   <dimension ref="A1:O226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -14733,7 +14736,7 @@
         <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>251</v>
@@ -27802,7 +27805,7 @@
   <dimension ref="A1:AJ28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="W25" sqref="W25:W26"/>
@@ -27850,76 +27853,76 @@
         <v>32</v>
       </c>
       <c r="E1" s="91" t="s">
+        <v>284</v>
+      </c>
+      <c r="F1" s="91" t="s">
         <v>285</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="G1" s="91" t="s">
         <v>286</v>
       </c>
-      <c r="G1" s="91" t="s">
-        <v>287</v>
-      </c>
       <c r="H1" s="92" t="s">
+        <v>289</v>
+      </c>
+      <c r="I1" s="92" t="s">
         <v>290</v>
       </c>
-      <c r="I1" s="92" t="s">
+      <c r="J1" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="N1" s="92" t="s">
         <v>293</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="N1" s="92" t="s">
-        <v>294</v>
-      </c>
       <c r="O1" s="92" t="s">
+        <v>295</v>
+      </c>
+      <c r="P1" s="92" t="s">
         <v>296</v>
       </c>
-      <c r="P1" s="92" t="s">
+      <c r="Q1" s="92" t="s">
         <v>297</v>
       </c>
-      <c r="Q1" s="92" t="s">
+      <c r="R1" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="92" t="s">
         <v>299</v>
       </c>
-      <c r="S1" s="92" t="s">
+      <c r="T1" s="92" t="s">
         <v>300</v>
       </c>
-      <c r="T1" s="92" t="s">
+      <c r="U1" s="92" t="s">
         <v>301</v>
       </c>
-      <c r="U1" s="92" t="s">
+      <c r="V1" s="92" t="s">
         <v>302</v>
       </c>
-      <c r="V1" s="92" t="s">
+      <c r="W1" s="92" t="s">
         <v>303</v>
       </c>
-      <c r="W1" s="92" t="s">
+      <c r="X1" s="92" t="s">
         <v>304</v>
       </c>
-      <c r="X1" s="92" t="s">
+      <c r="Y1" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>306</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>307</v>
       </c>
       <c r="AA1" s="4" t="s">
         <v>248</v>
       </c>
       <c r="AB1" s="92" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AC1" s="4" t="s">
         <v>191</v>
@@ -27937,10 +27940,10 @@
         <v>195</v>
       </c>
       <c r="AH1" s="97" t="s">
+        <v>317</v>
+      </c>
+      <c r="AI1" s="97" t="s">
         <v>318</v>
-      </c>
-      <c r="AI1" s="97" t="s">
-        <v>319</v>
       </c>
       <c r="AJ1" s="97" t="s">
         <v>27</v>
@@ -27948,7 +27951,7 @@
     </row>
     <row r="2" spans="1:36" customFormat="1">
       <c r="A2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -27957,13 +27960,13 @@
         <v>259</v>
       </c>
       <c r="D2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H2">
         <v>0.23</v>
@@ -28040,7 +28043,7 @@
     </row>
     <row r="3" spans="1:36" customFormat="1">
       <c r="A3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -28049,13 +28052,13 @@
         <v>259</v>
       </c>
       <c r="D3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H3">
         <v>0.28000000000000003</v>
@@ -28132,7 +28135,7 @@
     </row>
     <row r="4" spans="1:36" customFormat="1">
       <c r="A4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -28141,13 +28144,13 @@
         <v>259</v>
       </c>
       <c r="D4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H4">
         <v>0.33</v>
@@ -28222,12 +28225,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:36" customFormat="1">
       <c r="A5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -28236,13 +28239,13 @@
         <v>259</v>
       </c>
       <c r="D5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H5">
         <v>0.38</v>
@@ -28319,7 +28322,7 @@
     </row>
     <row r="6" spans="1:36" customFormat="1">
       <c r="A6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -28328,13 +28331,13 @@
         <v>259</v>
       </c>
       <c r="D6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E6" t="s">
         <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H6">
         <v>0.42</v>
@@ -28411,7 +28414,7 @@
     </row>
     <row r="7" spans="1:36" customFormat="1">
       <c r="A7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -28420,13 +28423,13 @@
         <v>259</v>
       </c>
       <c r="D7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E7" t="s">
         <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H7">
         <v>0.23</v>
@@ -28501,12 +28504,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ7" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8" spans="1:36" customFormat="1">
       <c r="A8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -28515,13 +28518,13 @@
         <v>259</v>
       </c>
       <c r="D8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E8" t="s">
         <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H8">
         <v>0.28000000000000003</v>
@@ -28596,12 +28599,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:36" customFormat="1">
       <c r="A9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -28610,13 +28613,13 @@
         <v>259</v>
       </c>
       <c r="D9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E9" t="s">
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H9">
         <v>0.38</v>
@@ -28691,12 +28694,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:36" customFormat="1">
       <c r="A10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -28705,13 +28708,13 @@
         <v>259</v>
       </c>
       <c r="D10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H10">
         <v>0.42</v>
@@ -28786,12 +28789,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:36" customFormat="1">
       <c r="A11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -28800,16 +28803,16 @@
         <v>260</v>
       </c>
       <c r="D11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E11" t="s">
         <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H11">
         <v>0.61</v>
@@ -28892,7 +28895,7 @@
     </row>
     <row r="12" spans="1:36" customFormat="1">
       <c r="A12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -28901,16 +28904,16 @@
         <v>260</v>
       </c>
       <c r="D12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E12" t="s">
         <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H12">
         <v>0.75</v>
@@ -28993,7 +28996,7 @@
     </row>
     <row r="13" spans="1:36" customFormat="1">
       <c r="A13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -29002,16 +29005,16 @@
         <v>260</v>
       </c>
       <c r="D13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E13" t="s">
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H13">
         <v>0.89</v>
@@ -29092,12 +29095,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:36" customFormat="1">
       <c r="A14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -29106,16 +29109,16 @@
         <v>260</v>
       </c>
       <c r="D14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H14">
         <v>0.92</v>
@@ -29198,7 +29201,7 @@
     </row>
     <row r="15" spans="1:36" customFormat="1">
       <c r="A15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -29207,16 +29210,16 @@
         <v>260</v>
       </c>
       <c r="D15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H15">
         <v>0.94</v>
@@ -29299,7 +29302,7 @@
     </row>
     <row r="16" spans="1:36" customFormat="1">
       <c r="A16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -29308,16 +29311,16 @@
         <v>260</v>
       </c>
       <c r="D16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E16" t="s">
         <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H16">
         <v>0.61</v>
@@ -29398,12 +29401,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ16" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17" spans="1:36" customFormat="1">
       <c r="A17" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -29412,16 +29415,16 @@
         <v>260</v>
       </c>
       <c r="D17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E17" t="s">
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H17">
         <v>0.75</v>
@@ -29502,12 +29505,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ17" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="18" spans="1:36" customFormat="1">
       <c r="A18" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -29516,16 +29519,16 @@
         <v>260</v>
       </c>
       <c r="D18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E18" t="s">
         <v>28</v>
       </c>
       <c r="F18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H18">
         <v>0.92</v>
@@ -29606,12 +29609,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:36" customFormat="1">
       <c r="A19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -29620,16 +29623,16 @@
         <v>260</v>
       </c>
       <c r="D19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E19" t="s">
         <v>28</v>
       </c>
       <c r="F19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H19">
         <v>0.94</v>
@@ -29710,12 +29713,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="20" spans="1:36" customFormat="1">
       <c r="A20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -29724,13 +29727,13 @@
         <v>261</v>
       </c>
       <c r="D20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E20" t="s">
         <v>28</v>
       </c>
       <c r="F20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H20">
         <v>0.81</v>
@@ -29807,7 +29810,7 @@
     </row>
     <row r="21" spans="1:36" customFormat="1">
       <c r="A21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -29816,13 +29819,13 @@
         <v>261</v>
       </c>
       <c r="D21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E21" t="s">
         <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H21">
         <v>0.86</v>
@@ -29899,7 +29902,7 @@
     </row>
     <row r="22" spans="1:36" customFormat="1">
       <c r="A22" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -29908,13 +29911,13 @@
         <v>261</v>
       </c>
       <c r="D22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E22" t="s">
         <v>28</v>
       </c>
       <c r="F22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H22">
         <v>0.91</v>
@@ -29989,12 +29992,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:36" customFormat="1">
       <c r="A23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -30003,13 +30006,13 @@
         <v>261</v>
       </c>
       <c r="D23" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E23" t="s">
         <v>28</v>
       </c>
       <c r="F23" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H23">
         <v>0.93</v>
@@ -30086,7 +30089,7 @@
     </row>
     <row r="24" spans="1:36" customFormat="1">
       <c r="A24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -30095,13 +30098,13 @@
         <v>261</v>
       </c>
       <c r="D24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E24" t="s">
         <v>28</v>
       </c>
       <c r="F24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H24">
         <v>0.95</v>
@@ -30178,7 +30181,7 @@
     </row>
     <row r="25" spans="1:36" customFormat="1">
       <c r="A25" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -30187,13 +30190,13 @@
         <v>261</v>
       </c>
       <c r="D25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E25" t="s">
         <v>28</v>
       </c>
       <c r="F25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H25">
         <v>0.81</v>
@@ -30268,12 +30271,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ25" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:36" customFormat="1">
       <c r="A26" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -30282,13 +30285,13 @@
         <v>261</v>
       </c>
       <c r="D26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E26" t="s">
         <v>28</v>
       </c>
       <c r="F26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H26">
         <v>0.86</v>
@@ -30363,12 +30366,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ26" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27" spans="1:36" customFormat="1">
       <c r="A27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -30377,13 +30380,13 @@
         <v>261</v>
       </c>
       <c r="D27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E27" t="s">
         <v>28</v>
       </c>
       <c r="F27" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H27">
         <v>0.93</v>
@@ -30458,12 +30461,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="28" spans="1:36" customFormat="1">
       <c r="A28" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -30472,13 +30475,13 @@
         <v>261</v>
       </c>
       <c r="D28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E28" t="s">
         <v>28</v>
       </c>
       <c r="F28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H28">
         <v>0.95</v>
@@ -30553,7 +30556,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -30572,10 +30575,10 @@
   <dimension ref="A1:AS9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AT10" sqref="AT10"/>
+      <selection pane="bottomRight" activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30598,103 +30601,103 @@
         <v>32</v>
       </c>
       <c r="E1" s="89" t="s">
+        <v>279</v>
+      </c>
+      <c r="F1" s="89" t="s">
         <v>280</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="G1" s="89" t="s">
         <v>281</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="H1" s="89" t="s">
         <v>282</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="I1" s="90" t="s">
         <v>283</v>
       </c>
-      <c r="I1" s="90" t="s">
+      <c r="J1" s="91" t="s">
         <v>284</v>
       </c>
-      <c r="J1" s="91" t="s">
+      <c r="K1" s="91" t="s">
         <v>285</v>
       </c>
-      <c r="K1" s="91" t="s">
+      <c r="L1" s="91" t="s">
         <v>286</v>
       </c>
-      <c r="L1" s="91" t="s">
+      <c r="M1" s="91" t="s">
         <v>287</v>
       </c>
-      <c r="M1" s="91" t="s">
+      <c r="N1" s="91" t="s">
         <v>288</v>
       </c>
-      <c r="N1" s="91" t="s">
+      <c r="O1" s="92" t="s">
         <v>289</v>
       </c>
-      <c r="O1" s="92" t="s">
+      <c r="P1" s="92" t="s">
         <v>290</v>
       </c>
-      <c r="P1" s="92" t="s">
+      <c r="Q1" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="92" t="s">
         <v>293</v>
       </c>
-      <c r="S1" s="92" t="s">
+      <c r="T1" s="92" t="s">
         <v>294</v>
       </c>
-      <c r="T1" s="92" t="s">
+      <c r="U1" s="92" t="s">
         <v>295</v>
       </c>
-      <c r="U1" s="92" t="s">
+      <c r="V1" s="92" t="s">
         <v>296</v>
       </c>
-      <c r="V1" s="92" t="s">
+      <c r="W1" s="92" t="s">
         <v>297</v>
       </c>
-      <c r="W1" s="92" t="s">
+      <c r="X1" s="92" t="s">
         <v>298</v>
       </c>
-      <c r="X1" s="92" t="s">
+      <c r="Y1" s="92" t="s">
         <v>299</v>
       </c>
-      <c r="Y1" s="92" t="s">
+      <c r="Z1" s="92" t="s">
         <v>300</v>
       </c>
-      <c r="Z1" s="92" t="s">
+      <c r="AA1" s="92" t="s">
         <v>301</v>
       </c>
-      <c r="AA1" s="92" t="s">
+      <c r="AB1" s="92" t="s">
         <v>302</v>
       </c>
-      <c r="AB1" s="92" t="s">
+      <c r="AC1" s="92" t="s">
         <v>303</v>
       </c>
-      <c r="AC1" s="92" t="s">
+      <c r="AD1" s="92" t="s">
         <v>304</v>
       </c>
-      <c r="AD1" s="92" t="s">
+      <c r="AE1" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="92" t="s">
         <v>309</v>
       </c>
-      <c r="AI1" s="92" t="s">
+      <c r="AJ1" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="AK1" s="4" t="s">
         <v>310</v>
-      </c>
-      <c r="AJ1" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="AK1" s="4" t="s">
-        <v>311</v>
       </c>
       <c r="AL1" s="4" t="s">
         <v>27</v>
@@ -30712,7 +30715,7 @@
         <v>193</v>
       </c>
       <c r="AQ1" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AR1" t="s">
         <v>194</v>
@@ -30740,10 +30743,10 @@
       <c r="H2" s="94"/>
       <c r="I2" s="94"/>
       <c r="J2" s="94" t="s">
+        <v>311</v>
+      </c>
+      <c r="K2" s="94" t="s">
         <v>312</v>
-      </c>
-      <c r="K2" s="94" t="s">
-        <v>313</v>
       </c>
       <c r="L2" s="94"/>
       <c r="M2" s="94"/>
@@ -30799,6 +30802,9 @@
         <v>4</v>
       </c>
       <c r="AK2" s="94"/>
+      <c r="AL2" t="s">
+        <v>353</v>
+      </c>
       <c r="AM2">
         <v>1</v>
       </c>
@@ -30815,7 +30821,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="AQ2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AR2">
         <v>30</v>
@@ -30843,10 +30849,10 @@
       <c r="H3" s="94"/>
       <c r="I3" s="94"/>
       <c r="J3" s="94" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L3" s="94"/>
       <c r="M3" s="94"/>
@@ -30899,7 +30905,9 @@
         <v>0</v>
       </c>
       <c r="AK3" s="94"/>
-      <c r="AL3" s="95"/>
+      <c r="AL3" t="s">
+        <v>353</v>
+      </c>
       <c r="AM3">
         <v>1</v>
       </c>
@@ -30916,7 +30924,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="AQ3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AR3">
         <v>30</v>
@@ -30939,10 +30947,10 @@
         <v>239</v>
       </c>
       <c r="J4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O4">
         <v>0.98</v>
@@ -30983,7 +30991,9 @@
       <c r="AI4">
         <v>0</v>
       </c>
-      <c r="AL4" s="95"/>
+      <c r="AL4" t="s">
+        <v>353</v>
+      </c>
       <c r="AM4">
         <v>1</v>
       </c>
@@ -30998,7 +31008,7 @@
         <v>9.4392925743255696E-2</v>
       </c>
       <c r="AQ4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AR4">
         <v>20</v>
@@ -31026,10 +31036,10 @@
       <c r="H5" s="86"/>
       <c r="I5" s="86"/>
       <c r="J5" s="86" t="s">
+        <v>313</v>
+      </c>
+      <c r="K5" s="86" t="s">
         <v>314</v>
-      </c>
-      <c r="K5" s="86" t="s">
-        <v>315</v>
       </c>
       <c r="L5" s="86"/>
       <c r="M5" s="86"/>
@@ -31085,7 +31095,9 @@
         <v>10</v>
       </c>
       <c r="AK5" s="86"/>
-      <c r="AL5" s="96"/>
+      <c r="AL5" t="s">
+        <v>353</v>
+      </c>
       <c r="AM5">
         <v>1</v>
       </c>
@@ -31102,7 +31114,7 @@
         <v>7.5009138873610326E-2</v>
       </c>
       <c r="AQ5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AR5">
         <v>40</v>
@@ -31130,10 +31142,10 @@
       <c r="H6" s="86"/>
       <c r="I6" s="86"/>
       <c r="J6" s="86" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K6" s="86" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L6" s="86"/>
       <c r="M6" s="86"/>
@@ -31186,7 +31198,9 @@
         <v>0</v>
       </c>
       <c r="AK6" s="86"/>
-      <c r="AL6" s="86"/>
+      <c r="AL6" t="s">
+        <v>353</v>
+      </c>
       <c r="AM6">
         <v>1</v>
       </c>
@@ -31203,7 +31217,7 @@
         <v>7.5009138873610326E-2</v>
       </c>
       <c r="AQ6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AR6">
         <v>40</v>
@@ -31226,13 +31240,13 @@
         <v>188</v>
       </c>
       <c r="G7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J7" s="96" t="s">
         <v>156</v>
       </c>
       <c r="K7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -31288,7 +31302,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="AQ7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AR7">
         <v>30</v>
@@ -31311,13 +31325,13 @@
         <v>189</v>
       </c>
       <c r="G8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J8" s="96" t="s">
         <v>156</v>
       </c>
       <c r="K8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -31373,7 +31387,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="AQ8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AR8">
         <v>30</v>
@@ -31402,7 +31416,7 @@
         <v>156</v>
       </c>
       <c r="K9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O9">
         <v>1</v>
@@ -31458,7 +31472,7 @@
         <v>7.5009138873610326E-2</v>
       </c>
       <c r="AQ9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AR9">
         <v>40</v>
@@ -31525,7 +31539,7 @@
         <v>193</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J1" t="s">
         <v>194</v>
@@ -31566,7 +31580,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="I2" s="85" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J2">
         <v>30</v>
@@ -31607,7 +31621,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="I3" s="85" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J3">
         <v>30</v>
@@ -31646,7 +31660,7 @@
         <v>9.4392925743255696E-2</v>
       </c>
       <c r="I4" s="85" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J4">
         <v>20</v>
@@ -31687,7 +31701,7 @@
         <v>7.5009138873610326E-2</v>
       </c>
       <c r="I5" s="85" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J5">
         <v>40</v>
@@ -31728,7 +31742,7 @@
         <v>7.5009138873610326E-2</v>
       </c>
       <c r="I6" s="85" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J6">
         <v>40</v>
@@ -31767,7 +31781,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="I7" s="85" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J7">
         <v>30</v>
@@ -31806,7 +31820,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="I8" s="85" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J8">
         <v>30</v>
@@ -31845,7 +31859,7 @@
         <v>7.5009138873610326E-2</v>
       </c>
       <c r="I9" s="85" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J9">
         <v>40</v>
@@ -31914,7 +31928,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E2">
         <f>'Matrix 2024'!D13</f>
@@ -31935,7 +31949,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E3">
         <f>'Matrix 2024'!E13</f>
@@ -31956,7 +31970,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E4">
         <f>'Matrix 2024'!F13</f>

</xml_diff>

<commit_message>
Update LWR CHP cV parameters and adjust investment/fixed costs accordingly
</commit_message>
<xml_diff>
--- a/src_files/data_files/gg-smr-scenario-changes.xlsx
+++ b/src_files/data_files/gg-smr-scenario-changes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\north_european_model\src_files\data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\backbone\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC328F0-5165-4EF8-8CA6-02D9BFB1C28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16AEE4D-B3FA-48F0-8971-6A4BC18E114A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="862" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="17880" windowWidth="29040" windowHeight="15720" tabRatio="862" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="20" r:id="rId1"/>
@@ -63,7 +63,7 @@
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStatic" hidden="1">0</definedName>
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStaticPercentile" hidden="1">0.5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">TEMPLATE!$A$1:$G$346</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">unittypedata_nuclear!$A$1:$AJ$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">unittypedata_nuclear!$A$1:$AL$1</definedName>
     <definedName name="a">#REF!</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aaa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
@@ -315,7 +315,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3474" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3476" uniqueCount="358">
   <si>
     <t>Country</t>
   </si>
@@ -1404,7 +1404,16 @@
     <t>DEA data</t>
   </si>
   <si>
-    <t>2025-10-09</t>
+    <t>unitSize_input1</t>
+  </si>
+  <si>
+    <t>unitSize_output1</t>
+  </si>
+  <si>
+    <t>unitSize_output2</t>
+  </si>
+  <si>
+    <t>2025-10-15</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1426,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="43">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1717,8 +1726,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1823,6 +1840,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -1936,7 +1958,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -1953,8 +1975,9 @@
     <xf numFmtId="0" fontId="35" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="42" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2176,6 +2199,7 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="13"/>
     <xf numFmtId="0" fontId="41" fillId="18" borderId="9" xfId="12"/>
+    <xf numFmtId="0" fontId="42" fillId="19" borderId="9" xfId="14"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -2204,8 +2228,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="Bad" xfId="11" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="14" builtinId="22"/>
     <cellStyle name="ČEPS" xfId="3" xr:uid="{055F4603-C55C-4D73-9C89-501612CA5A5D}"/>
     <cellStyle name="Comma" xfId="10" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="4" xr:uid="{4D01FCE7-C6F2-4A9A-8B9B-FBFD721CF21A}"/>
@@ -4193,8 +4218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFA71A91-038D-4743-9A24-5EE3CD503F37}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4233,7 +4258,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5736,31 +5761,31 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="E3" s="105" t="s">
+      <c r="E3" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="106"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="104"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
       <c r="E4" s="68" t="s">
         <v>146</v>
       </c>
@@ -5790,20 +5815,20 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="104"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="106" t="s">
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="107"/>
+      <c r="L5" s="107"/>
+      <c r="M5" s="107"/>
     </row>
     <row r="6" spans="1:13">
       <c r="B6" s="69">
@@ -14470,16 +14495,16 @@
       </c>
     </row>
     <row r="348" spans="1:17">
-      <c r="J348" s="107" t="s">
+      <c r="J348" s="108" t="s">
         <v>200</v>
       </c>
-      <c r="K348" s="107"/>
-      <c r="L348" s="107"/>
-      <c r="M348" s="107" t="s">
+      <c r="K348" s="108"/>
+      <c r="L348" s="108"/>
+      <c r="M348" s="108" t="s">
         <v>233</v>
       </c>
-      <c r="N348" s="107"/>
-      <c r="O348" s="107"/>
+      <c r="N348" s="108"/>
+      <c r="O348" s="108"/>
       <c r="Q348" t="s">
         <v>234</v>
       </c>
@@ -27802,13 +27827,13 @@
   <sheetPr>
     <tabColor theme="6" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:AJ28"/>
+  <dimension ref="A1:AL28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W25" sqref="W25:W26"/>
+      <selection pane="bottomRight" activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -27831,15 +27856,15 @@
     <col min="20" max="20" width="14" style="97" customWidth="1"/>
     <col min="21" max="21" width="14.7109375" style="97" customWidth="1"/>
     <col min="22" max="22" width="14.5703125" style="97" customWidth="1"/>
-    <col min="23" max="27" width="8.42578125" style="97" customWidth="1"/>
-    <col min="28" max="28" width="14" style="97" customWidth="1"/>
-    <col min="29" max="35" width="10.140625" style="97" customWidth="1"/>
-    <col min="36" max="1031" width="8.42578125" style="97"/>
-    <col min="1032" max="1032" width="9.140625" style="97" customWidth="1"/>
-    <col min="1033" max="16384" width="8.42578125" style="97"/>
+    <col min="23" max="29" width="8.42578125" style="97" customWidth="1"/>
+    <col min="30" max="30" width="14" style="97" customWidth="1"/>
+    <col min="31" max="37" width="10.140625" style="97" customWidth="1"/>
+    <col min="38" max="1033" width="8.42578125" style="97"/>
+    <col min="1034" max="1034" width="9.140625" style="97" customWidth="1"/>
+    <col min="1035" max="16384" width="8.42578125" style="97"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="48" customHeight="1">
+    <row r="1" spans="1:38" ht="48" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -27919,37 +27944,43 @@
         <v>306</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="AB1" s="92" t="s">
+        <v>355</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="AD1" s="92" t="s">
         <v>309</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="AG1" s="97" t="s">
+      <c r="AI1" s="97" t="s">
         <v>195</v>
       </c>
-      <c r="AH1" s="97" t="s">
+      <c r="AJ1" s="97" t="s">
         <v>317</v>
       </c>
-      <c r="AI1" s="97" t="s">
+      <c r="AK1" s="97" t="s">
         <v>318</v>
       </c>
-      <c r="AJ1" s="97" t="s">
+      <c r="AL1" s="97" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:36" customFormat="1">
+    <row r="2" spans="1:38" customFormat="1">
       <c r="A2" t="s">
         <v>319</v>
       </c>
@@ -28022,26 +28053,26 @@
       <c r="AA2" s="98">
         <v>1</v>
       </c>
-      <c r="AB2">
+      <c r="AD2">
         <v>300</v>
       </c>
-      <c r="AC2">
+      <c r="AE2">
         <v>30000</v>
       </c>
-      <c r="AD2">
+      <c r="AF2">
         <v>1350000</v>
       </c>
-      <c r="AE2">
+      <c r="AG2">
         <v>7.5009138873610326E-2</v>
       </c>
-      <c r="AF2">
+      <c r="AH2">
         <v>40</v>
       </c>
-      <c r="AG2">
+      <c r="AI2">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:36" customFormat="1">
+    <row r="3" spans="1:38" customFormat="1">
       <c r="A3" t="s">
         <v>320</v>
       </c>
@@ -28114,26 +28145,26 @@
       <c r="AA3" s="98">
         <v>1</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>400</v>
       </c>
-      <c r="AC3">
+      <c r="AE3">
         <v>114150</v>
       </c>
-      <c r="AD3">
+      <c r="AF3">
         <v>4425000</v>
       </c>
-      <c r="AE3">
+      <c r="AG3">
         <v>7.2459849539607671E-2</v>
       </c>
-      <c r="AF3">
+      <c r="AH3">
         <v>50</v>
       </c>
-      <c r="AG3">
+      <c r="AI3">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:36" customFormat="1">
+    <row r="4" spans="1:38" customFormat="1">
       <c r="A4" t="s">
         <v>321</v>
       </c>
@@ -28206,29 +28237,29 @@
       <c r="AA4" s="98">
         <v>1</v>
       </c>
-      <c r="AB4">
+      <c r="AD4">
         <v>500</v>
       </c>
-      <c r="AC4">
+      <c r="AE4">
         <v>198300</v>
       </c>
-      <c r="AD4">
+      <c r="AF4">
         <v>7500000</v>
       </c>
-      <c r="AE4">
+      <c r="AG4">
         <v>7.122922550001945E-2</v>
       </c>
-      <c r="AF4">
+      <c r="AH4">
         <v>60</v>
       </c>
-      <c r="AG4">
+      <c r="AI4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AL4" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="5" spans="1:36" customFormat="1">
+    <row r="5" spans="1:38" customFormat="1">
       <c r="A5" t="s">
         <v>322</v>
       </c>
@@ -28301,26 +28332,26 @@
       <c r="AA5" s="98">
         <v>1</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <v>1250</v>
       </c>
-      <c r="AC5">
+      <c r="AE5">
         <v>374150</v>
       </c>
-      <c r="AD5">
+      <c r="AF5">
         <v>17250000</v>
       </c>
-      <c r="AE5">
+      <c r="AG5">
         <v>7.0619527184264883E-2</v>
       </c>
-      <c r="AF5">
+      <c r="AH5">
         <v>70</v>
       </c>
-      <c r="AG5">
+      <c r="AI5">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:36" customFormat="1">
+    <row r="6" spans="1:38" customFormat="1">
       <c r="A6" t="s">
         <v>323</v>
       </c>
@@ -28393,26 +28424,26 @@
       <c r="AA6" s="98">
         <v>1</v>
       </c>
-      <c r="AB6">
+      <c r="AD6">
         <v>2000</v>
       </c>
-      <c r="AC6">
+      <c r="AE6">
         <v>550000</v>
       </c>
-      <c r="AD6">
+      <c r="AF6">
         <v>27000000</v>
       </c>
-      <c r="AE6">
+      <c r="AG6">
         <v>7.0313571760871663E-2</v>
       </c>
-      <c r="AF6">
+      <c r="AH6">
         <v>80</v>
       </c>
-      <c r="AG6">
+      <c r="AI6">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:36" customFormat="1">
+    <row r="7" spans="1:38" customFormat="1">
       <c r="A7" t="s">
         <v>347</v>
       </c>
@@ -28485,29 +28516,29 @@
       <c r="AA7" s="98">
         <v>1</v>
       </c>
-      <c r="AB7">
+      <c r="AD7">
         <v>2000</v>
       </c>
-      <c r="AC7">
+      <c r="AE7">
         <v>550000</v>
       </c>
-      <c r="AD7">
+      <c r="AF7">
         <v>27000000</v>
       </c>
-      <c r="AE7">
+      <c r="AG7">
         <v>7.5009138873610326E-2</v>
       </c>
-      <c r="AF7">
+      <c r="AH7">
         <v>40</v>
       </c>
-      <c r="AG7">
+      <c r="AI7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AL7" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="8" spans="1:36" customFormat="1">
+    <row r="8" spans="1:38" customFormat="1">
       <c r="A8" t="s">
         <v>349</v>
       </c>
@@ -28580,29 +28611,29 @@
       <c r="AA8" s="98">
         <v>1</v>
       </c>
-      <c r="AB8">
+      <c r="AD8">
         <v>1250</v>
       </c>
-      <c r="AC8">
+      <c r="AE8">
         <v>374150</v>
       </c>
-      <c r="AD8">
+      <c r="AF8">
         <v>17250000</v>
       </c>
-      <c r="AE8">
+      <c r="AG8">
         <v>7.2459849539607671E-2</v>
       </c>
-      <c r="AF8">
+      <c r="AH8">
         <v>50</v>
       </c>
-      <c r="AG8">
+      <c r="AI8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ8" t="s">
+      <c r="AL8" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:36" customFormat="1">
+    <row r="9" spans="1:38" customFormat="1">
       <c r="A9" t="s">
         <v>324</v>
       </c>
@@ -28675,29 +28706,29 @@
       <c r="AA9" s="98">
         <v>1</v>
       </c>
-      <c r="AB9">
+      <c r="AD9">
         <v>400</v>
       </c>
-      <c r="AC9">
+      <c r="AE9">
         <v>114150</v>
       </c>
-      <c r="AD9">
+      <c r="AF9">
         <v>4425000</v>
       </c>
-      <c r="AE9">
+      <c r="AG9">
         <v>7.0619527184264883E-2</v>
       </c>
-      <c r="AF9">
+      <c r="AH9">
         <v>70</v>
       </c>
-      <c r="AG9">
+      <c r="AI9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ9" t="s">
+      <c r="AL9" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="10" spans="1:36" customFormat="1">
+    <row r="10" spans="1:38" customFormat="1">
       <c r="A10" t="s">
         <v>326</v>
       </c>
@@ -28770,29 +28801,29 @@
       <c r="AA10" s="98">
         <v>1</v>
       </c>
-      <c r="AB10">
+      <c r="AD10">
         <v>300</v>
       </c>
-      <c r="AC10">
+      <c r="AE10">
         <v>30000</v>
       </c>
-      <c r="AD10">
+      <c r="AF10">
         <v>1350000</v>
       </c>
-      <c r="AE10">
+      <c r="AG10">
         <v>7.0313571760871663E-2</v>
       </c>
-      <c r="AF10">
+      <c r="AH10">
         <v>80</v>
       </c>
-      <c r="AG10">
+      <c r="AI10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ10" t="s">
+      <c r="AL10" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="11" spans="1:36" customFormat="1">
+    <row r="11" spans="1:38" customFormat="1">
       <c r="A11" t="s">
         <v>319</v>
       </c>
@@ -28829,8 +28860,8 @@
       <c r="L11">
         <v>0.2</v>
       </c>
-      <c r="M11" s="98">
-        <v>0</v>
+      <c r="M11">
+        <v>-0.17</v>
       </c>
       <c r="N11">
         <v>1.2</v>
@@ -28874,26 +28905,34 @@
       <c r="AA11" s="98">
         <v>1</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="99">
+        <f>ROUNDUP(AA11/L11,0)</f>
+        <v>5</v>
+      </c>
+      <c r="AC11" s="99">
+        <f>ROUNDUP(SUM(AA11:AB11)/H11,0)</f>
+        <v>10</v>
+      </c>
+      <c r="AD11">
         <v>300</v>
       </c>
-      <c r="AC11">
-        <v>30000</v>
-      </c>
-      <c r="AD11">
-        <v>1350000</v>
-      </c>
       <c r="AE11">
+        <v>16216</v>
+      </c>
+      <c r="AF11">
+        <v>729729</v>
+      </c>
+      <c r="AG11">
         <v>7.5009138873610326E-2</v>
       </c>
-      <c r="AF11">
+      <c r="AH11">
         <v>40</v>
       </c>
-      <c r="AG11">
+      <c r="AI11">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:36" customFormat="1">
+    <row r="12" spans="1:38" customFormat="1">
       <c r="A12" t="s">
         <v>320</v>
       </c>
@@ -28930,8 +28969,8 @@
       <c r="L12">
         <v>0.3</v>
       </c>
-      <c r="M12" s="98">
-        <v>0</v>
+      <c r="M12">
+        <v>-0.16</v>
       </c>
       <c r="N12">
         <v>2.08</v>
@@ -28975,26 +29014,34 @@
       <c r="AA12" s="98">
         <v>1</v>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="99">
+        <f>ROUNDUP(AA12/L12,0)</f>
+        <v>4</v>
+      </c>
+      <c r="AC12" s="99">
+        <f t="shared" ref="AC12:AC19" si="0">ROUNDUP(SUM(AA12:AB12)/H12,0)</f>
+        <v>7</v>
+      </c>
+      <c r="AD12">
         <v>427.5</v>
       </c>
-      <c r="AC12">
-        <v>125056</v>
-      </c>
-      <c r="AD12">
-        <v>4837500</v>
-      </c>
       <c r="AE12">
+        <v>88149</v>
+      </c>
+      <c r="AF12">
+        <v>3392137</v>
+      </c>
+      <c r="AG12">
         <v>7.2459849539607671E-2</v>
       </c>
-      <c r="AF12">
+      <c r="AH12">
         <v>50</v>
       </c>
-      <c r="AG12">
+      <c r="AI12">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:36" customFormat="1">
+    <row r="13" spans="1:38" customFormat="1">
       <c r="A13" t="s">
         <v>321</v>
       </c>
@@ -29031,8 +29078,8 @@
       <c r="L13">
         <v>0.4</v>
       </c>
-      <c r="M13" s="98">
-        <v>0</v>
+      <c r="M13">
+        <v>-0.15</v>
       </c>
       <c r="N13">
         <v>2.96</v>
@@ -29076,29 +29123,37 @@
       <c r="AA13" s="98">
         <v>1</v>
       </c>
-      <c r="AB13">
+      <c r="AB13" s="99">
+        <f t="shared" ref="AB13:AB19" si="1">ROUNDUP(AA13/L13,0)</f>
+        <v>3</v>
+      </c>
+      <c r="AC13" s="99">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AD13">
         <v>555</v>
       </c>
-      <c r="AC13">
-        <v>220113</v>
-      </c>
-      <c r="AD13">
-        <v>8325000</v>
-      </c>
       <c r="AE13">
+        <v>160082</v>
+      </c>
+      <c r="AF13">
+        <v>6054545</v>
+      </c>
+      <c r="AG13">
         <v>7.122922550001945E-2</v>
       </c>
-      <c r="AF13">
+      <c r="AH13">
         <v>60</v>
       </c>
-      <c r="AG13">
+      <c r="AI13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ13" t="s">
+      <c r="AL13" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="14" spans="1:36" customFormat="1">
+    <row r="14" spans="1:38" customFormat="1">
       <c r="A14" t="s">
         <v>322</v>
       </c>
@@ -29135,8 +29190,8 @@
       <c r="L14">
         <v>0.5</v>
       </c>
-      <c r="M14" s="98">
-        <v>0</v>
+      <c r="M14">
+        <v>-0.14000000000000001</v>
       </c>
       <c r="N14">
         <v>11.49</v>
@@ -29180,26 +29235,34 @@
       <c r="AA14" s="98">
         <v>1</v>
       </c>
-      <c r="AB14">
+      <c r="AB14" s="99">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AC14" s="99">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AD14">
         <v>1497.5</v>
       </c>
-      <c r="AC14">
-        <v>445557</v>
-      </c>
-      <c r="AD14">
-        <v>20632500</v>
-      </c>
       <c r="AE14">
+        <v>355794</v>
+      </c>
+      <c r="AF14">
+        <v>16564259</v>
+      </c>
+      <c r="AG14">
         <v>7.0619527184264883E-2</v>
       </c>
-      <c r="AF14">
+      <c r="AH14">
         <v>70</v>
       </c>
-      <c r="AG14">
+      <c r="AI14">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:36" customFormat="1">
+    <row r="15" spans="1:38" customFormat="1">
       <c r="A15" t="s">
         <v>323</v>
       </c>
@@ -29236,8 +29299,8 @@
       <c r="L15">
         <v>0.6</v>
       </c>
-      <c r="M15" s="98">
-        <v>0</v>
+      <c r="M15">
+        <v>-0.13</v>
       </c>
       <c r="N15">
         <v>20.010000000000002</v>
@@ -29281,26 +29344,34 @@
       <c r="AA15" s="98">
         <v>1</v>
       </c>
-      <c r="AB15">
+      <c r="AB15" s="99">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AC15" s="99">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AD15">
         <v>2440</v>
       </c>
-      <c r="AC15">
-        <v>671000</v>
-      </c>
-      <c r="AD15">
-        <v>32940000</v>
-      </c>
       <c r="AE15">
+        <v>551506</v>
+      </c>
+      <c r="AF15">
+        <v>27073972</v>
+      </c>
+      <c r="AG15">
         <v>7.0313571760871663E-2</v>
       </c>
-      <c r="AF15">
+      <c r="AH15">
         <v>80</v>
       </c>
-      <c r="AG15">
+      <c r="AI15">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:36" customFormat="1">
+    <row r="16" spans="1:38" customFormat="1">
       <c r="A16" t="s">
         <v>347</v>
       </c>
@@ -29337,8 +29408,8 @@
       <c r="L16">
         <v>0.2</v>
       </c>
-      <c r="M16" s="98">
-        <v>0</v>
+      <c r="M16">
+        <v>-0.17</v>
       </c>
       <c r="N16">
         <v>20.010000000000002</v>
@@ -29382,29 +29453,37 @@
       <c r="AA16" s="98">
         <v>1</v>
       </c>
-      <c r="AB16">
+      <c r="AB16" s="99">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AC16" s="99">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AD16">
         <v>2440</v>
       </c>
-      <c r="AC16">
-        <v>671000</v>
-      </c>
-      <c r="AD16">
-        <v>32940000</v>
-      </c>
       <c r="AE16">
+        <v>551506</v>
+      </c>
+      <c r="AF16">
+        <v>27073972</v>
+      </c>
+      <c r="AG16">
         <v>7.5009138873610326E-2</v>
       </c>
-      <c r="AF16">
+      <c r="AH16">
         <v>40</v>
       </c>
-      <c r="AG16">
+      <c r="AI16">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ16" t="s">
+      <c r="AL16" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="17" spans="1:36" customFormat="1">
+    <row r="17" spans="1:38" customFormat="1">
       <c r="A17" t="s">
         <v>349</v>
       </c>
@@ -29441,8 +29520,8 @@
       <c r="L17">
         <v>0.3</v>
       </c>
-      <c r="M17" s="98">
-        <v>0</v>
+      <c r="M17">
+        <v>-0.16</v>
       </c>
       <c r="N17">
         <v>11.49</v>
@@ -29486,29 +29565,37 @@
       <c r="AA17" s="98">
         <v>1</v>
       </c>
-      <c r="AB17">
+      <c r="AB17" s="99">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AC17" s="99">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AD17">
         <v>1497.5</v>
       </c>
-      <c r="AC17">
-        <v>445557</v>
-      </c>
-      <c r="AD17">
-        <v>20632500</v>
-      </c>
       <c r="AE17">
+        <v>355794</v>
+      </c>
+      <c r="AF17">
+        <v>16564259</v>
+      </c>
+      <c r="AG17">
         <v>7.2459849539607671E-2</v>
       </c>
-      <c r="AF17">
+      <c r="AH17">
         <v>50</v>
       </c>
-      <c r="AG17">
+      <c r="AI17">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ17" t="s">
+      <c r="AL17" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="18" spans="1:36" customFormat="1">
+    <row r="18" spans="1:38" customFormat="1">
       <c r="A18" t="s">
         <v>324</v>
       </c>
@@ -29545,8 +29632,8 @@
       <c r="L18">
         <v>0.5</v>
       </c>
-      <c r="M18" s="98">
-        <v>0</v>
+      <c r="M18">
+        <v>-0.14000000000000001</v>
       </c>
       <c r="N18">
         <v>2.08</v>
@@ -29590,29 +29677,37 @@
       <c r="AA18" s="98">
         <v>1</v>
       </c>
-      <c r="AB18">
+      <c r="AB18" s="99">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AC18" s="99">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AD18">
         <v>427.5</v>
       </c>
-      <c r="AC18">
-        <v>125056</v>
-      </c>
-      <c r="AD18">
-        <v>4837500</v>
-      </c>
       <c r="AE18">
+        <v>88149</v>
+      </c>
+      <c r="AF18">
+        <v>3392137</v>
+      </c>
+      <c r="AG18">
         <v>7.0619527184264883E-2</v>
       </c>
-      <c r="AF18">
+      <c r="AH18">
         <v>70</v>
       </c>
-      <c r="AG18">
+      <c r="AI18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AL18" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="19" spans="1:36" customFormat="1">
+    <row r="19" spans="1:38" customFormat="1">
       <c r="A19" t="s">
         <v>326</v>
       </c>
@@ -29649,8 +29744,8 @@
       <c r="L19">
         <v>0.6</v>
       </c>
-      <c r="M19" s="98">
-        <v>0</v>
+      <c r="M19">
+        <v>-0.13</v>
       </c>
       <c r="N19">
         <v>1.2</v>
@@ -29694,29 +29789,37 @@
       <c r="AA19" s="98">
         <v>1</v>
       </c>
-      <c r="AB19">
+      <c r="AB19" s="99">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AC19" s="99">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AD19">
         <v>300</v>
       </c>
-      <c r="AC19">
-        <v>30000</v>
-      </c>
-      <c r="AD19">
-        <v>1350000</v>
-      </c>
       <c r="AE19">
+        <v>16216</v>
+      </c>
+      <c r="AF19">
+        <v>729729</v>
+      </c>
+      <c r="AG19">
         <v>7.0313571760871663E-2</v>
       </c>
-      <c r="AF19">
+      <c r="AH19">
         <v>80</v>
       </c>
-      <c r="AG19">
+      <c r="AI19">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ19" t="s">
+      <c r="AL19" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="20" spans="1:36" customFormat="1">
+    <row r="20" spans="1:38" customFormat="1">
       <c r="A20" t="s">
         <v>319</v>
       </c>
@@ -29789,26 +29892,26 @@
       <c r="AA20" s="98">
         <v>1</v>
       </c>
-      <c r="AB20">
+      <c r="AD20">
         <v>50</v>
       </c>
-      <c r="AC20">
+      <c r="AE20">
         <v>7320</v>
       </c>
-      <c r="AD20">
+      <c r="AF20">
         <v>244000</v>
       </c>
-      <c r="AE20">
+      <c r="AG20">
         <v>7.5009138873610326E-2</v>
       </c>
-      <c r="AF20">
+      <c r="AH20">
         <v>40</v>
       </c>
-      <c r="AG20">
+      <c r="AI20">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:36" customFormat="1">
+    <row r="21" spans="1:38" customFormat="1">
       <c r="A21" t="s">
         <v>320</v>
       </c>
@@ -29881,26 +29984,26 @@
       <c r="AA21" s="98">
         <v>1</v>
       </c>
-      <c r="AB21">
+      <c r="AD21">
         <v>150</v>
       </c>
-      <c r="AC21">
+      <c r="AE21">
         <v>20160</v>
       </c>
-      <c r="AD21">
+      <c r="AF21">
         <v>611000</v>
       </c>
-      <c r="AE21">
+      <c r="AG21">
         <v>7.2459849539607671E-2</v>
       </c>
-      <c r="AF21">
+      <c r="AH21">
         <v>50</v>
       </c>
-      <c r="AG21">
+      <c r="AI21">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:36" customFormat="1">
+    <row r="22" spans="1:38" customFormat="1">
       <c r="A22" t="s">
         <v>321</v>
       </c>
@@ -29973,29 +30076,29 @@
       <c r="AA22" s="98">
         <v>1</v>
       </c>
-      <c r="AB22">
+      <c r="AD22">
         <v>250</v>
       </c>
-      <c r="AC22">
+      <c r="AE22">
         <v>33000</v>
       </c>
-      <c r="AD22">
+      <c r="AF22">
         <v>978000</v>
       </c>
-      <c r="AE22">
+      <c r="AG22">
         <v>7.122922550001945E-2</v>
       </c>
-      <c r="AF22">
+      <c r="AH22">
         <v>60</v>
       </c>
-      <c r="AG22">
+      <c r="AI22">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ22" t="s">
+      <c r="AL22" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="23" spans="1:36" customFormat="1">
+    <row r="23" spans="1:38" customFormat="1">
       <c r="A23" t="s">
         <v>322</v>
       </c>
@@ -30068,26 +30171,26 @@
       <c r="AA23" s="98">
         <v>1</v>
       </c>
-      <c r="AB23">
+      <c r="AD23">
         <v>625</v>
       </c>
-      <c r="AC23">
+      <c r="AE23">
         <v>50250</v>
       </c>
-      <c r="AD23">
+      <c r="AF23">
         <v>1614000</v>
       </c>
-      <c r="AE23">
+      <c r="AG23">
         <v>7.0619527184264883E-2</v>
       </c>
-      <c r="AF23">
+      <c r="AH23">
         <v>70</v>
       </c>
-      <c r="AG23">
+      <c r="AI23">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:36" customFormat="1">
+    <row r="24" spans="1:38" customFormat="1">
       <c r="A24" t="s">
         <v>323</v>
       </c>
@@ -30160,26 +30263,26 @@
       <c r="AA24" s="98">
         <v>1</v>
       </c>
-      <c r="AB24">
+      <c r="AD24">
         <v>1000</v>
       </c>
-      <c r="AC24">
+      <c r="AE24">
         <v>67500</v>
       </c>
-      <c r="AD24">
+      <c r="AF24">
         <v>2250000</v>
       </c>
-      <c r="AE24">
+      <c r="AG24">
         <v>7.0313571760871663E-2</v>
       </c>
-      <c r="AF24">
+      <c r="AH24">
         <v>80</v>
       </c>
-      <c r="AG24">
+      <c r="AI24">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:36" customFormat="1">
+    <row r="25" spans="1:38" customFormat="1">
       <c r="A25" t="s">
         <v>347</v>
       </c>
@@ -30252,29 +30355,29 @@
       <c r="AA25" s="98">
         <v>1</v>
       </c>
-      <c r="AB25">
+      <c r="AD25">
         <v>1000</v>
       </c>
-      <c r="AC25">
+      <c r="AE25">
         <v>67500</v>
       </c>
-      <c r="AD25">
+      <c r="AF25">
         <v>2250000</v>
       </c>
-      <c r="AE25">
+      <c r="AG25">
         <v>7.5009138873610326E-2</v>
       </c>
-      <c r="AF25">
+      <c r="AH25">
         <v>40</v>
       </c>
-      <c r="AG25">
+      <c r="AI25">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ25" t="s">
+      <c r="AL25" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="26" spans="1:36" customFormat="1">
+    <row r="26" spans="1:38" customFormat="1">
       <c r="A26" t="s">
         <v>349</v>
       </c>
@@ -30347,29 +30450,29 @@
       <c r="AA26" s="98">
         <v>1</v>
       </c>
-      <c r="AB26">
+      <c r="AD26">
         <v>625</v>
       </c>
-      <c r="AC26">
+      <c r="AE26">
         <v>50250</v>
       </c>
-      <c r="AD26">
+      <c r="AF26">
         <v>1614000</v>
       </c>
-      <c r="AE26">
+      <c r="AG26">
         <v>7.2459849539607671E-2</v>
       </c>
-      <c r="AF26">
+      <c r="AH26">
         <v>50</v>
       </c>
-      <c r="AG26">
+      <c r="AI26">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ26" t="s">
+      <c r="AL26" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="27" spans="1:36" customFormat="1">
+    <row r="27" spans="1:38" customFormat="1">
       <c r="A27" t="s">
         <v>324</v>
       </c>
@@ -30442,29 +30545,29 @@
       <c r="AA27" s="98">
         <v>1</v>
       </c>
-      <c r="AB27">
+      <c r="AD27">
         <v>150</v>
       </c>
-      <c r="AC27">
+      <c r="AE27">
         <v>20160</v>
       </c>
-      <c r="AD27">
+      <c r="AF27">
         <v>611000</v>
       </c>
-      <c r="AE27">
+      <c r="AG27">
         <v>7.0619527184264883E-2</v>
       </c>
-      <c r="AF27">
+      <c r="AH27">
         <v>70</v>
       </c>
-      <c r="AG27">
+      <c r="AI27">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ27" t="s">
+      <c r="AL27" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="28" spans="1:36" customFormat="1">
+    <row r="28" spans="1:38" customFormat="1">
       <c r="A28" t="s">
         <v>326</v>
       </c>
@@ -30537,30 +30640,30 @@
       <c r="AA28" s="98">
         <v>1</v>
       </c>
-      <c r="AB28">
+      <c r="AD28">
         <v>50</v>
       </c>
-      <c r="AC28">
+      <c r="AE28">
         <v>7320</v>
       </c>
-      <c r="AD28">
+      <c r="AF28">
         <v>244000</v>
       </c>
-      <c r="AE28">
+      <c r="AG28">
         <v>7.0313571760871663E-2</v>
       </c>
-      <c r="AF28">
+      <c r="AH28">
         <v>80</v>
       </c>
-      <c r="AG28">
+      <c r="AI28">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ28" t="s">
+      <c r="AL28" t="s">
         <v>327</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AL1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -32668,20 +32771,20 @@
       </c>
     </row>
     <row r="2" spans="2:12" ht="14.45" customHeight="1">
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="101" t="s">
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="102" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="14.45" customHeight="1">
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="102"/>
     </row>
     <row r="4" spans="2:12" ht="15" customHeight="1">
       <c r="B4" s="22" t="s">
@@ -32751,7 +32854,7 @@
       <c r="G6" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="H6" s="102"/>
+      <c r="H6" s="103"/>
     </row>
     <row r="7" spans="2:12" ht="26.1" customHeight="1">
       <c r="B7" s="33" t="s">
@@ -32772,7 +32875,7 @@
       <c r="G7" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="99"/>
+      <c r="H7" s="100"/>
     </row>
     <row r="8" spans="2:12" ht="15.75" customHeight="1">
       <c r="B8" s="29" t="s">
@@ -32793,7 +32896,7 @@
       <c r="G8" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="99"/>
+      <c r="H8" s="100"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" customHeight="1">
       <c r="B9" s="29" t="s">
@@ -32814,7 +32917,7 @@
       <c r="G9" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="103"/>
+      <c r="H9" s="104"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" customHeight="1">
       <c r="B10" s="35" t="s">
@@ -32838,7 +32941,7 @@
       <c r="G10" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="102"/>
+      <c r="H10" s="103"/>
     </row>
     <row r="11" spans="2:12" ht="15.75" customHeight="1">
       <c r="B11" s="35" t="s">
@@ -32862,7 +32965,7 @@
       <c r="G11" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="99"/>
+      <c r="H11" s="100"/>
       <c r="J11">
         <f>E11/D11</f>
         <v>0.89873417721518989</v>
@@ -32894,7 +32997,7 @@
       <c r="G12" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="H12" s="99"/>
+      <c r="H12" s="100"/>
       <c r="J12" s="37"/>
     </row>
     <row r="13" spans="2:12" ht="15.75" customHeight="1">
@@ -32919,7 +33022,7 @@
       <c r="G13" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="103"/>
+      <c r="H13" s="104"/>
     </row>
     <row r="14" spans="2:12" ht="15.75" customHeight="1">
       <c r="B14" s="35" t="s">
@@ -32943,7 +33046,7 @@
       <c r="G14" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="H14" s="102"/>
+      <c r="H14" s="103"/>
     </row>
     <row r="15" spans="2:12" ht="15.75" customHeight="1">
       <c r="B15" s="38" t="s">
@@ -32964,7 +33067,7 @@
       <c r="G15" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="H15" s="103"/>
+      <c r="H15" s="104"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" customHeight="1">
       <c r="B16" s="29" t="s">
@@ -33219,10 +33322,10 @@
       </c>
     </row>
     <row r="31" spans="2:12">
-      <c r="I31" s="99"/>
+      <c r="I31" s="100"/>
     </row>
     <row r="32" spans="2:12">
-      <c r="I32" s="99"/>
+      <c r="I32" s="100"/>
     </row>
     <row r="33" spans="2:11">
       <c r="D33">
@@ -33234,7 +33337,7 @@
       <c r="F33">
         <v>2050</v>
       </c>
-      <c r="I33" s="99"/>
+      <c r="I33" s="100"/>
     </row>
     <row r="34" spans="2:11">
       <c r="B34" t="s">

</xml_diff>